<commit_message>
More files for match prediction
</commit_message>
<xml_diff>
--- a/epaSheet.xlsx
+++ b/epaSheet.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsstudent\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Teams</t>
   </si>
@@ -31,28 +39,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -172,38 +167,22 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -212,24 +191,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -355,7 +395,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -364,7 +404,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -373,7 +413,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -447,7 +487,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -455,7 +495,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -474,7 +514,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -504,7 +544,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -530,7 +570,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -556,7 +596,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -582,7 +622,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -608,7 +648,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -634,7 +674,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -660,7 +700,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -686,7 +726,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -712,7 +752,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -725,9 +765,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -742,7 +788,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="38000"/>
             </a:srgbClr>
@@ -750,7 +796,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -769,7 +815,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -795,7 +841,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -821,7 +867,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -847,7 +893,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -873,7 +919,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -899,7 +945,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -925,7 +971,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -951,7 +997,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -977,7 +1023,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1003,7 +1049,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1016,9 +1062,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1032,7 +1084,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1051,7 +1103,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1081,7 +1133,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1107,7 +1159,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1133,7 +1185,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1159,7 +1211,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1185,7 +1237,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1211,7 +1263,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1237,7 +1289,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1263,7 +1315,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1289,7 +1341,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1302,52 +1354,59 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1328" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1094" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.0547" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6172" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.3516" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1" customWidth="1"/>
+    <col min="2" max="3" width="10.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
+    <row r="1" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" t="s" s="3">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s" s="3">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s" s="3">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s" s="3">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="13.55" customHeight="1">
+    <row r="2" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -1358,7 +1417,7 @@
         <v>57.41</v>
       </c>
       <c r="D2" s="6">
-        <v>18.99</v>
+        <v>18.989999999999998</v>
       </c>
       <c r="E2" s="6">
         <v>27.81</v>
@@ -1367,7 +1426,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="3" ht="13.55" customHeight="1">
+    <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1387,7 +1446,7 @@
         <v>7.44</v>
       </c>
     </row>
-    <row r="4" ht="13.55" customHeight="1">
+    <row r="4" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -1407,7 +1466,7 @@
         <v>8.27</v>
       </c>
     </row>
-    <row r="5" ht="13.55" customHeight="1">
+    <row r="5" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -1427,7 +1486,7 @@
         <v>7.77</v>
       </c>
     </row>
-    <row r="6" ht="13.55" customHeight="1">
+    <row r="6" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -1447,7 +1506,7 @@
         <v>5.97</v>
       </c>
     </row>
-    <row r="7" ht="13.55" customHeight="1">
+    <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1467,7 +1526,7 @@
         <v>7.36</v>
       </c>
     </row>
-    <row r="8" ht="13.55" customHeight="1">
+    <row r="8" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -1487,7 +1546,7 @@
         <v>7.56</v>
       </c>
     </row>
-    <row r="9" ht="13.55" customHeight="1">
+    <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -1501,13 +1560,13 @@
         <v>5.97</v>
       </c>
       <c r="E9" s="8">
-        <v>8.550000000000001</v>
+        <v>8.5500000000000007</v>
       </c>
       <c r="F9" s="8">
         <v>8.69</v>
       </c>
     </row>
-    <row r="10" ht="13.55" customHeight="1">
+    <row r="10" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -1527,7 +1586,7 @@
         <v>5.12</v>
       </c>
     </row>
-    <row r="11" ht="13.55" customHeight="1">
+    <row r="11" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -1547,7 +1606,7 @@
         <v>2.09</v>
       </c>
     </row>
-    <row r="12" ht="13.55" customHeight="1">
+    <row r="12" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -1567,7 +1626,7 @@
         <v>7.78</v>
       </c>
     </row>
-    <row r="13" ht="13.55" customHeight="1">
+    <row r="13" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -1575,7 +1634,7 @@
         <v>4639</v>
       </c>
       <c r="C13" s="8">
-        <v>20.31</v>
+        <v>20.309999999999999</v>
       </c>
       <c r="D13" s="8">
         <v>3.02</v>
@@ -1587,7 +1646,7 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="14" ht="13.55" customHeight="1">
+    <row r="14" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -1595,10 +1654,10 @@
         <v>4587</v>
       </c>
       <c r="C14" s="8">
-        <v>19.4</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="D14" s="8">
-        <v>4.48</v>
+        <v>4.4800000000000004</v>
       </c>
       <c r="E14" s="8">
         <v>11.16</v>
@@ -1607,7 +1666,7 @@
         <v>3.76</v>
       </c>
     </row>
-    <row r="15" ht="13.55" customHeight="1">
+    <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -1627,7 +1686,7 @@
         <v>7.03</v>
       </c>
     </row>
-    <row r="16" ht="13.55" customHeight="1">
+    <row r="16" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -1647,7 +1706,7 @@
         <v>6.38</v>
       </c>
     </row>
-    <row r="17" ht="13.55" customHeight="1">
+    <row r="17" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -1655,7 +1714,7 @@
         <v>8879</v>
       </c>
       <c r="C17" s="8">
-        <v>16.94</v>
+        <v>16.940000000000001</v>
       </c>
       <c r="D17" s="8">
         <v>5.98</v>
@@ -1667,7 +1726,7 @@
         <v>4.78</v>
       </c>
     </row>
-    <row r="18" ht="13.55" customHeight="1">
+    <row r="18" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -1687,7 +1746,7 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="19" ht="13.55" customHeight="1">
+    <row r="19" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -1707,7 +1766,7 @@
         <v>7.39</v>
       </c>
     </row>
-    <row r="20" ht="13.55" customHeight="1">
+    <row r="20" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -1727,7 +1786,7 @@
         <v>2.73</v>
       </c>
     </row>
-    <row r="21" ht="13.55" customHeight="1">
+    <row r="21" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -1741,13 +1800,13 @@
         <v>6.1</v>
       </c>
       <c r="E21" s="8">
-        <v>4.81</v>
+        <v>4.8099999999999996</v>
       </c>
       <c r="F21" s="8">
-        <v>4.61</v>
-      </c>
-    </row>
-    <row r="22" ht="13.55" customHeight="1">
+        <v>4.6100000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -1767,7 +1826,7 @@
         <v>3.91</v>
       </c>
     </row>
-    <row r="23" ht="13.55" customHeight="1">
+    <row r="23" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -1787,7 +1846,7 @@
         <v>4.01</v>
       </c>
     </row>
-    <row r="24" ht="13.55" customHeight="1">
+    <row r="24" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -1807,7 +1866,7 @@
         <v>3.86</v>
       </c>
     </row>
-    <row r="25" ht="13.55" customHeight="1">
+    <row r="25" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -1827,7 +1886,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="26" ht="13.55" customHeight="1">
+    <row r="26" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -1838,7 +1897,7 @@
         <v>12.36</v>
       </c>
       <c r="D26" s="8">
-        <v>4.94</v>
+        <v>4.9400000000000004</v>
       </c>
       <c r="E26" s="8">
         <v>4.41</v>
@@ -1847,7 +1906,7 @@
         <v>3.01</v>
       </c>
     </row>
-    <row r="27" ht="13.55" customHeight="1">
+    <row r="27" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -1867,7 +1926,7 @@
         <v>2.15</v>
       </c>
     </row>
-    <row r="28" ht="13.55" customHeight="1">
+    <row r="28" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -1887,7 +1946,7 @@
         <v>-0.05</v>
       </c>
     </row>
-    <row r="29" ht="13.55" customHeight="1">
+    <row r="29" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -1907,7 +1966,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="30" ht="13.55" customHeight="1">
+    <row r="30" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -1927,7 +1986,7 @@
         <v>6.14</v>
       </c>
     </row>
-    <row r="31" ht="13.55" customHeight="1">
+    <row r="31" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -1947,7 +2006,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="32" ht="13.55" customHeight="1">
+    <row r="32" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -1967,7 +2026,7 @@
         <v>3.87</v>
       </c>
     </row>
-    <row r="33" ht="13.55" customHeight="1">
+    <row r="33" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -1975,19 +2034,19 @@
         <v>7091</v>
       </c>
       <c r="C33" s="8">
-        <v>8.880000000000001</v>
+        <v>8.8800000000000008</v>
       </c>
       <c r="D33" s="8">
         <v>2.83</v>
       </c>
       <c r="E33" s="8">
-        <v>-1.11</v>
+        <v>-1.1100000000000001</v>
       </c>
       <c r="F33" s="8">
         <v>7.17</v>
       </c>
     </row>
-    <row r="34" ht="13.55" customHeight="1">
+    <row r="34" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>32</v>
       </c>
@@ -2007,7 +2066,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="35" ht="13.55" customHeight="1">
+    <row r="35" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>33</v>
       </c>
@@ -2029,7 +2088,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>